<commit_message>
updated land use files (and io, but those may change)
</commit_message>
<xml_diff>
--- a/InputData/elec/BDPbES/BAU Dispatch Priority by Elec Source.xlsx
+++ b/InputData/elec/BDPbES/BAU Dispatch Priority by Elec Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/elec/bdpbes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\All_states_RMI\LA\elec\BDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE96AA19-DDB0-8C47-A24E-4E08B95FA730}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACDD59B0-BB96-481F-9746-1F96242D1183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="23000" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6910" yWindow="880" windowWidth="18690" windowHeight="11930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Notes:</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Priority Order (dimensionless)</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
   </si>
 </sst>
 </file>
@@ -497,44 +500,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
       <c r="C1" s="4">
-        <v>44307</v>
+        <v>44463</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -552,15 +558,17 @@
   </sheetPr>
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="22.6328125" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -673,7 +681,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -821,7 +829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -969,7 +977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1265,303 +1273,303 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1709,7 +1717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1857,7 +1865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2005,7 +2013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2153,7 +2161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2301,7 +2309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2449,7 +2457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2597,7 +2605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2745,7 +2753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2893,7 +2901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>22</v>
       </c>

</xml_diff>